<commit_message>
updated vegan version in yml file
</commit_message>
<xml_diff>
--- a/results/tables/PERMANOVA.xlsx
+++ b/results/tables/PERMANOVA.xlsx
@@ -352,7 +352,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -393,54 +393,98 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model</t>
+          <t>level</t>
         </is>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>6.174145186147887</v>
+        <v>0.7852985403925928</v>
       </c>
       <c r="D2">
-        <v>0.5428347900420263</v>
+        <v>0.06904394947671905</v>
       </c>
       <c r="E2">
-        <v>1.682140144982229</v>
+        <v>1.283723165649595</v>
       </c>
       <c r="F2">
-        <v>0.0001</v>
+        <v>0.0062</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Residual</t>
+          <t>site</t>
         </is>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>5.199748490913387</v>
+        <v>2.188545411289753</v>
       </c>
       <c r="D3">
-        <v>0.4571652099579737</v>
+        <v>0.1924183110400957</v>
+      </c>
+      <c r="E3">
+        <v>2.385068691748097</v>
+      </c>
+      <c r="F3">
+        <v>0.0001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>site:plant</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>3.20030123446554</v>
+      </c>
+      <c r="D4">
+        <v>0.2813725295252116</v>
+      </c>
+      <c r="E4">
+        <v>1.49471847617761</v>
+      </c>
+      <c r="F4">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Residual</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>5.199748490913387</v>
+      </c>
+      <c r="D5">
+        <v>0.4571652099579737</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>29</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>11.37389367706127</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>1</v>
       </c>
     </row>
@@ -451,7 +495,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -492,54 +536,98 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Model</t>
+          <t>level</t>
         </is>
       </c>
       <c r="B2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>6.006756450521212</v>
+        <v>0.4728651059065685</v>
       </c>
       <c r="D2">
-        <v>0.5750454360463336</v>
+        <v>0.04526884405202474</v>
       </c>
       <c r="E2">
-        <v>1.917023065916434</v>
+        <v>0.9054736837328426</v>
       </c>
       <c r="F2">
-        <v>0.0001</v>
+        <v>0.7792</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Residual</t>
+          <t>site</t>
         </is>
       </c>
       <c r="B3">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C3">
-        <v>4.438951095338217</v>
+        <v>2.466256733236879</v>
       </c>
       <c r="D3">
-        <v>0.4249545639536665</v>
+        <v>0.2361024107184082</v>
+      </c>
+      <c r="E3">
+        <v>3.148368729800303</v>
+      </c>
+      <c r="F3">
+        <v>0.0001</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>site:plant</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>3.067634611377764</v>
+      </c>
+      <c r="D4">
+        <v>0.2936741812759006</v>
+      </c>
+      <c r="E4">
+        <v>1.678317604875803</v>
+      </c>
+      <c r="F4">
+        <v>0.0001</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Residual</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>4.438951095338217</v>
+      </c>
+      <c r="D5">
+        <v>0.4249545639536665</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B4">
+      <c r="B6">
         <v>29</v>
       </c>
-      <c r="C4">
+      <c r="C6">
         <v>10.44570754585943</v>
       </c>
-      <c r="D4">
+      <c r="D6">
         <v>1</v>
       </c>
     </row>

</xml_diff>